<commit_message>
Fixed bad value in auxiliary that was preventing reads. Bug fixes to atmos and lbl code. Need to again check lbl units, as taus are ~15000 times too large.
git-svn-id: file:///mnt/svn/rtmath@138 1d52797c-35fc-48e8-8e80-2db72aa187e2
</commit_message>
<xml_diff>
--- a/rtmath/profiles.xlsx
+++ b/rtmath/profiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="6795" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="6795" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TRP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="46">
   <si>
     <t>Profile</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>USS</t>
-  </si>
-  <si>
-    <t>2..59e-6</t>
   </si>
   <si>
     <t>TRP+Aux</t>
@@ -9705,8 +9702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView topLeftCell="K17" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AC53"/>
+    <sheetView tabSelected="1" topLeftCell="K17" workbookViewId="0">
+      <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11397,8 +11394,8 @@
       <c r="Z20" s="1">
         <v>2.9399999999999998E-6</v>
       </c>
-      <c r="AA20" t="s">
-        <v>45</v>
+      <c r="AA20" s="1">
+        <v>2.5900000000000002E-6</v>
       </c>
       <c r="AB20" s="1">
         <v>2.14E-4</v>
@@ -14353,8 +14350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD21" sqref="AD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14364,7 +14361,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -16219,8 +16216,8 @@
       <c r="AC20" s="1">
         <v>2.9399999999999998E-6</v>
       </c>
-      <c r="AD20" t="s">
-        <v>45</v>
+      <c r="AD20" s="1">
+        <v>2.5900000000000002E-6</v>
       </c>
       <c r="AE20" s="1">
         <v>2.14E-4</v>

</xml_diff>

<commit_message>
And MSVC builds agree with Linux gcc! But, I must test the modifications again against gcc. Still must solve tau scaling bug, but will use a limited H2O-only profile for speed.
git-svn-id: file:///mnt/svn/rtmath@143 1d52797c-35fc-48e8-8e80-2db72aa187e2
</commit_message>
<xml_diff>
--- a/rtmath/profiles.xlsx
+++ b/rtmath/profiles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="6795" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15180" windowHeight="6795" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TRP" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="USS" sheetId="6" r:id="rId6"/>
     <sheet name="Auxiliary" sheetId="7" r:id="rId7"/>
     <sheet name="TRP+Aux" sheetId="8" r:id="rId8"/>
+    <sheet name="TRP+H2O" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="47">
   <si>
     <t>Profile</t>
   </si>
@@ -159,6 +160,9 @@
   </si>
   <si>
     <t>TRP+Aux</t>
+  </si>
+  <si>
+    <t>TRP-H2O</t>
   </si>
 </sst>
 </file>
@@ -511,7 +515,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection sqref="A1:I53"/>
+      <selection sqref="A1:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9702,7 +9706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" workbookViewId="0">
+    <sheetView topLeftCell="K17" workbookViewId="0">
       <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
@@ -19463,4 +19467,911 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1013</v>
+      </c>
+      <c r="C4">
+        <v>299.7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.45E+19</v>
+      </c>
+      <c r="E4" s="1">
+        <v>25900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>904</v>
+      </c>
+      <c r="C5">
+        <v>293.7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.231E+19</v>
+      </c>
+      <c r="E5" s="1">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>805</v>
+      </c>
+      <c r="C6">
+        <v>287.7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.028E+19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>715</v>
+      </c>
+      <c r="C7">
+        <v>283.7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.827E+19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>633</v>
+      </c>
+      <c r="C8">
+        <v>277</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.656E+19</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>559</v>
+      </c>
+      <c r="C9">
+        <v>270.3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.499E+19</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>492</v>
+      </c>
+      <c r="C10">
+        <v>263.60000000000002</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.353E+19</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>432</v>
+      </c>
+      <c r="C11">
+        <v>257</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.218E+19</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>378</v>
+      </c>
+      <c r="C12">
+        <v>250.3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.095E+19</v>
+      </c>
+      <c r="E12" s="1">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>329</v>
+      </c>
+      <c r="C13">
+        <v>243.6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9.789E+18</v>
+      </c>
+      <c r="E13" s="1">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>286</v>
+      </c>
+      <c r="C14">
+        <v>237</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.747E+18</v>
+      </c>
+      <c r="E14" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>247</v>
+      </c>
+      <c r="C15">
+        <v>230.1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7.78E+18</v>
+      </c>
+      <c r="E15" s="1">
+        <v>73.099999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>213</v>
+      </c>
+      <c r="C16">
+        <v>223.6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.904E+18</v>
+      </c>
+      <c r="E16" s="1">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>182</v>
+      </c>
+      <c r="C17">
+        <v>217</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6.079E+18</v>
+      </c>
+      <c r="E17" s="1">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>156</v>
+      </c>
+      <c r="C18">
+        <v>210.3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5.377E+18</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>132</v>
+      </c>
+      <c r="C19">
+        <v>203.7</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4.697E+18</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>111</v>
+      </c>
+      <c r="C20">
+        <v>197</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4.084E+18</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>93.7</v>
+      </c>
+      <c r="C21">
+        <v>194.8</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.486E+18</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="C22">
+        <v>198.8</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2.877E+18</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="C23">
+        <v>202.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.381E+18</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>56.5</v>
+      </c>
+      <c r="C24">
+        <v>206.7</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.981E+18</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>210.7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.651E+18</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>40.9</v>
+      </c>
+      <c r="C26">
+        <v>214.6</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.381E+18</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>35</v>
+      </c>
+      <c r="C27">
+        <v>217</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.169E+18</v>
+      </c>
+      <c r="E27" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>219.2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9.92E+17</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>25.7</v>
+      </c>
+      <c r="C29">
+        <v>221.4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8.413E+17</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27.5</v>
+      </c>
+      <c r="B30">
+        <v>17.63</v>
+      </c>
+      <c r="C30">
+        <v>227</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5.623E+17</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>12.2</v>
+      </c>
+      <c r="C31">
+        <v>232.3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>3.807E+17</v>
+      </c>
+      <c r="E31" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32.5</v>
+      </c>
+      <c r="B32">
+        <v>8.52</v>
+      </c>
+      <c r="C32">
+        <v>237.7</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2.598E+17</v>
+      </c>
+      <c r="E32" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>243.1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.789E+17</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>37.5</v>
+      </c>
+      <c r="B34">
+        <v>4.26</v>
+      </c>
+      <c r="C34">
+        <v>248.5</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.243E+17</v>
+      </c>
+      <c r="E34" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>3.05</v>
+      </c>
+      <c r="C35">
+        <v>254</v>
+      </c>
+      <c r="D35" s="1">
+        <v>8.703E+16</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>42.5</v>
+      </c>
+      <c r="B36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C36">
+        <v>259.39999999999998</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6.147E+16</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>1.59</v>
+      </c>
+      <c r="C37">
+        <v>264.8</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4.352E+16</v>
+      </c>
+      <c r="E37" s="1">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>47.5</v>
+      </c>
+      <c r="B38">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C38">
+        <v>269.60000000000002</v>
+      </c>
+      <c r="D38" s="1">
+        <v>3.119E+16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="C39">
+        <v>270.2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2.291E+16</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="C40">
+        <v>263.39999999999998</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1.255E+16</v>
+      </c>
+      <c r="E40" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>60</v>
+      </c>
+      <c r="B41">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="C41">
+        <v>253.1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>6844000000000000</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>65</v>
+      </c>
+      <c r="B42">
+        <v>0.121</v>
+      </c>
+      <c r="C42">
+        <v>236</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3716000000000000</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>70</v>
+      </c>
+      <c r="B43">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C43">
+        <v>218.9</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1920000000000000</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>75</v>
+      </c>
+      <c r="B44">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C44">
+        <v>201.8</v>
+      </c>
+      <c r="D44" s="1">
+        <v>933800000000000</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C45">
+        <v>184.8</v>
+      </c>
+      <c r="D45" s="1">
+        <v>431400000000000</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="C46">
+        <v>177.1</v>
+      </c>
+      <c r="D46" s="1">
+        <v>180100000000000</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>90</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1.72E-3</v>
+      </c>
+      <c r="C47">
+        <v>177</v>
+      </c>
+      <c r="D47" s="1">
+        <v>70430000000000</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>95</v>
+      </c>
+      <c r="B48" s="1">
+        <v>6.8800000000000003E-4</v>
+      </c>
+      <c r="C48">
+        <v>184.3</v>
+      </c>
+      <c r="D48" s="1">
+        <v>27060000000000</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2.8899999999999998E-4</v>
+      </c>
+      <c r="C49">
+        <v>190.7</v>
+      </c>
+      <c r="D49" s="1">
+        <v>10980000000000</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>105</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="C50">
+        <v>212</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4445000000000</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>110</v>
+      </c>
+      <c r="B51" s="1">
+        <v>6.4700000000000001E-5</v>
+      </c>
+      <c r="C51">
+        <v>241.6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1941000000000</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>115</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="C52">
+        <v>299.7</v>
+      </c>
+      <c r="D52" s="1">
+        <v>870600000000</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>120</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2.2500000000000001E-5</v>
+      </c>
+      <c r="C53">
+        <v>380</v>
+      </c>
+      <c r="D53" s="1">
+        <v>422500000000</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>